<commit_message>
revised examples for a new solver
</commit_message>
<xml_diff>
--- a/volcanic_test/CA_CP_selectivity/reaction_data.xlsx
+++ b/volcanic_test/CA_CP_selectivity/reaction_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\pregabalin\RF\spectre\volcanic_test\C\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\pregabalin\RF\spectre\volcanic_test\CA_CP_selectivity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BE38C4-862A-48CE-82F0-D350C2AFA667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD903D50-BB51-409F-99B4-91E66E35231C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{0DD04FB3-EBB0-4954-9900-17133E5A11EF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>INT1</t>
   </si>
@@ -222,13 +222,16 @@
   </si>
   <si>
     <t>productB</t>
+  </si>
+  <si>
+    <t>Catalyst</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,8 +246,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,6 +273,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -270,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -278,8 +303,39 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -596,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F3C747A-0ACD-4395-86BB-8CAB535DA314}">
-  <dimension ref="A1:U43"/>
+  <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,6 +664,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -659,7 +718,7 @@
       <c r="R1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="8" t="s">
         <v>58</v>
       </c>
       <c r="T1" s="1" t="s">
@@ -724,7 +783,7 @@
       <c r="R2" s="2">
         <v>18.303197096016913</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="9">
         <v>-8.9966037015430818</v>
       </c>
       <c r="T2" s="2">
@@ -735,67 +794,67 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4">
-        <v>27.629243285012969</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="B3" s="15">
+        <v>0</v>
+      </c>
+      <c r="C3" s="16">
+        <v>27.629243285012969</v>
+      </c>
+      <c r="D3" s="16">
         <v>6.5631218605518304</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="16">
         <v>13.111811002568761</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="16">
         <v>10.593615379220051</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="16">
         <v>29.992444062181661</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="16">
         <v>2.6430700141754886</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="16">
         <v>16.121346564675086</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="16">
         <v>6.7143516501693883</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="16">
         <v>10.207697036481628</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="16">
         <v>-49.363662326927624</v>
       </c>
-      <c r="M3" s="4">
-        <v>-68.489999999999995</v>
-      </c>
-      <c r="N3" s="4">
+      <c r="M3" s="16">
+        <v>-68.489999999999995</v>
+      </c>
+      <c r="N3" s="16">
         <v>31.040384926961412</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O3" s="16">
         <v>18.449802140446376</v>
       </c>
-      <c r="P3" s="4">
+      <c r="P3" s="16">
         <v>41.55116905210523</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="Q3" s="16">
         <v>13.469491417664457</v>
       </c>
-      <c r="R3" s="4">
+      <c r="R3" s="16">
         <v>30.539004836514501</v>
       </c>
-      <c r="S3" s="4">
+      <c r="S3" s="16">
         <v>-1.2550189968313816E-2</v>
       </c>
-      <c r="T3" s="4">
+      <c r="T3" s="16">
         <v>6.2186191451368806</v>
       </c>
-      <c r="U3" s="3">
+      <c r="U3" s="15">
         <v>-62.54</v>
       </c>
     </row>
@@ -854,7 +913,7 @@
       <c r="R4" s="2">
         <v>34.309081912983508</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4" s="9">
         <v>7.307348127813027</v>
       </c>
       <c r="T4" s="2">
@@ -919,7 +978,7 @@
       <c r="R5" s="2">
         <v>38.921904247037567</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S5" s="9">
         <v>5.5176910334803857</v>
       </c>
       <c r="T5" s="2">
@@ -984,7 +1043,7 @@
       <c r="R6" s="2">
         <v>33.717340453908669</v>
       </c>
-      <c r="S6" s="2">
+      <c r="S6" s="9">
         <v>1.9509270353541339</v>
       </c>
       <c r="T6" s="2">
@@ -1049,7 +1108,7 @@
       <c r="R7" s="2">
         <v>31.751353190592557</v>
       </c>
-      <c r="S7" s="2">
+      <c r="S7" s="9">
         <v>-3.3082300839229122</v>
       </c>
       <c r="T7" s="2">
@@ -1114,7 +1173,7 @@
       <c r="R8" s="2">
         <v>22.39769658366621</v>
       </c>
-      <c r="S8" s="2">
+      <c r="S8" s="9">
         <v>-4.9535599931919068</v>
       </c>
       <c r="T8" s="2">
@@ -1179,7 +1238,7 @@
       <c r="R9" s="2">
         <v>26.362301604216047</v>
       </c>
-      <c r="S9" s="2">
+      <c r="S9" s="9">
         <v>2.2565241617246317</v>
       </c>
       <c r="T9" s="2">
@@ -1244,7 +1303,7 @@
       <c r="R10" s="2">
         <v>35.754863800757562</v>
       </c>
-      <c r="S10" s="2">
+      <c r="S10" s="9">
         <v>3.4952279154495423</v>
       </c>
       <c r="T10" s="2">
@@ -1309,7 +1368,7 @@
       <c r="R11" s="2">
         <v>41.718086579111841</v>
       </c>
-      <c r="S11" s="2">
+      <c r="S11" s="9">
         <v>11.93648570896857</v>
       </c>
       <c r="T11" s="2">
@@ -1374,7 +1433,7 @@
       <c r="R12" s="2">
         <v>37.665630227642374</v>
       </c>
-      <c r="S12" s="2">
+      <c r="S12" s="9">
         <v>10.623735834858644</v>
       </c>
       <c r="T12" s="2">
@@ -1439,7 +1498,7 @@
       <c r="R13" s="2">
         <v>33.714830415915003</v>
       </c>
-      <c r="S13" s="2">
+      <c r="S13" s="9">
         <v>12.093990592856889</v>
       </c>
       <c r="T13" s="2">
@@ -1504,7 +1563,7 @@
       <c r="R14" s="2">
         <v>26.175303773830851</v>
       </c>
-      <c r="S14" s="2">
+      <c r="S14" s="9">
         <v>5.0025057336402936</v>
       </c>
       <c r="T14" s="2">
@@ -1569,7 +1628,7 @@
       <c r="R15" s="2">
         <v>36.785234399296314</v>
       </c>
-      <c r="S15" s="2">
+      <c r="S15" s="9">
         <v>4.4609650355801378</v>
       </c>
       <c r="T15" s="2">
@@ -1580,67 +1639,67 @@
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2">
-        <v>27.629243285012969</v>
-      </c>
-      <c r="D16" s="2">
+      <c r="B16" s="6">
+        <v>0</v>
+      </c>
+      <c r="C16" s="7">
+        <v>27.629243285012969</v>
+      </c>
+      <c r="D16" s="7">
         <v>2.9919652958653291</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="7">
         <v>3.4456546647180044</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="7">
         <v>-5.0872195165684682</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="7">
         <v>6.4733880019216885</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="7">
         <v>-12.124738559063994</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="7">
         <v>0.21398073945912757</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="7">
         <v>-6.3911842575578932</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="7">
         <v>10.107923025876834</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16" s="7">
         <v>-56.411849030824875</v>
       </c>
-      <c r="M16" s="2">
-        <v>-68.489999999999995</v>
-      </c>
-      <c r="N16" s="2">
+      <c r="M16" s="7">
+        <v>-68.489999999999995</v>
+      </c>
+      <c r="N16" s="7">
         <v>27.019304050983443</v>
       </c>
-      <c r="O16" s="2">
+      <c r="O16" s="7">
         <v>9.110138995199156</v>
       </c>
-      <c r="P16" s="2">
+      <c r="P16" s="7">
         <v>26.910744907400833</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="Q16" s="7">
         <v>2.2056958924243002</v>
       </c>
-      <c r="R16" s="2">
+      <c r="R16" s="7">
         <v>8.297558118453173</v>
       </c>
-      <c r="S16" s="2">
+      <c r="S16" s="10">
         <v>-31.164004298648678</v>
       </c>
-      <c r="T16" s="2">
+      <c r="T16" s="7">
         <v>-19.255756517037476</v>
       </c>
-      <c r="U16">
+      <c r="U16" s="6">
         <v>-62.54</v>
       </c>
     </row>
@@ -1699,7 +1758,7 @@
       <c r="R17" s="2">
         <v>18.321394871684987</v>
       </c>
-      <c r="S17" s="2">
+      <c r="S17" s="9">
         <v>-23.012655893255022</v>
       </c>
       <c r="T17" s="2">
@@ -1764,7 +1823,7 @@
       <c r="R18" s="2">
         <v>20.36644833222951</v>
       </c>
-      <c r="S18" s="2">
+      <c r="S18" s="9">
         <v>-16.824784714039886</v>
       </c>
       <c r="T18" s="2">
@@ -1829,7 +1888,7 @@
       <c r="R19" s="2">
         <v>24.78035015535713</v>
       </c>
-      <c r="S19" s="2">
+      <c r="S19" s="9">
         <v>-17.633016949996804</v>
       </c>
       <c r="T19" s="2">
@@ -1894,7 +1953,7 @@
       <c r="R20" s="2">
         <v>18.257388902418548</v>
       </c>
-      <c r="S20" s="2">
+      <c r="S20" s="9">
         <v>-23.175808363128461</v>
       </c>
       <c r="T20" s="2">
@@ -1959,7 +2018,7 @@
       <c r="R21" s="2">
         <v>18.365320536716762</v>
       </c>
-      <c r="S21" s="2">
+      <c r="S21" s="9">
         <v>-27.449775567752685</v>
       </c>
       <c r="T21" s="2">
@@ -1970,67 +2029,67 @@
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22" s="2">
-        <v>27.629243285012969</v>
-      </c>
-      <c r="D22" s="2">
+      <c r="B22" s="4">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5">
+        <v>27.629243285012969</v>
+      </c>
+      <c r="D22" s="5">
         <v>3.9219343752282865</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="5">
         <v>5.8458785022218853</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="5">
         <v>-3.4011014899737928</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="5">
         <v>13.532242367506027</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="5">
         <v>-8.3766243153962296</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="5">
         <v>4.8311956406441494</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22" s="5">
         <v>-5.7203766018253512</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="5">
         <v>19.243206327069164</v>
       </c>
-      <c r="L22" s="2">
+      <c r="L22" s="5">
         <v>-56.436949411046861</v>
       </c>
-      <c r="M22" s="2">
-        <v>-68.489999999999995</v>
-      </c>
-      <c r="N22" s="2">
+      <c r="M22" s="5">
+        <v>-68.489999999999995</v>
+      </c>
+      <c r="N22" s="5">
         <v>29.323518935158386</v>
       </c>
-      <c r="O22" s="2">
+      <c r="O22" s="5">
         <v>10.436982732730531</v>
       </c>
-      <c r="P22" s="2">
+      <c r="P22" s="5">
         <v>29.512399294538206</v>
       </c>
-      <c r="Q22" s="2">
+      <c r="Q22" s="5">
         <v>4.5795643309947218</v>
       </c>
-      <c r="R22" s="2">
+      <c r="R22" s="5">
         <v>10.815753742087242</v>
       </c>
-      <c r="S22" s="2">
+      <c r="S22" s="3">
         <v>-30.135516228105796</v>
       </c>
-      <c r="T22" s="2">
+      <c r="T22" s="5">
         <v>-17.698277937832035</v>
       </c>
-      <c r="U22">
+      <c r="U22" s="4">
         <v>-62.54</v>
       </c>
     </row>
@@ -2089,7 +2148,7 @@
       <c r="R23" s="2">
         <v>19.445891895984843</v>
       </c>
-      <c r="S23" s="2">
+      <c r="S23" s="9">
         <v>-17.27784657289477</v>
       </c>
       <c r="T23" s="2">
@@ -2154,7 +2213,7 @@
       <c r="R24" s="2">
         <v>22.855778518793777</v>
       </c>
-      <c r="S24" s="2">
+      <c r="S24" s="9">
         <v>-19.598376704171198</v>
       </c>
       <c r="T24" s="2">
@@ -2219,7 +2278,7 @@
       <c r="R25" s="2">
         <v>26.173421244978908</v>
       </c>
-      <c r="S25" s="2">
+      <c r="S25" s="9">
         <v>-13.73241789785733</v>
       </c>
       <c r="T25" s="2">
@@ -2284,7 +2343,7 @@
       <c r="R26" s="2">
         <v>27.46609081513953</v>
       </c>
-      <c r="S26" s="2">
+      <c r="S26" s="9">
         <v>-15.886030501841788</v>
       </c>
       <c r="T26" s="2">
@@ -2349,7 +2408,7 @@
       <c r="R27" s="2">
         <v>19.551941001145757</v>
       </c>
-      <c r="S27" s="2">
+      <c r="S27" s="9">
         <v>-18.414893786592227</v>
       </c>
       <c r="T27" s="2">
@@ -2414,7 +2473,7 @@
       <c r="R28" s="2">
         <v>12.800566290498503</v>
       </c>
-      <c r="S28" s="2">
+      <c r="S28" s="9">
         <v>-22.276587249972607</v>
       </c>
       <c r="T28" s="2">
@@ -2479,7 +2538,7 @@
       <c r="R29" s="2">
         <v>21.273827068793427</v>
       </c>
-      <c r="S29" s="2">
+      <c r="S29" s="9">
         <v>-20.526463254682209</v>
       </c>
       <c r="T29" s="2">
@@ -2493,64 +2552,64 @@
       <c r="A30" t="s">
         <v>39</v>
       </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30" s="2">
-        <v>27.629243285012969</v>
-      </c>
-      <c r="D30" s="2">
+      <c r="B30" s="11">
+        <v>0</v>
+      </c>
+      <c r="C30" s="12">
+        <v>27.629243285012969</v>
+      </c>
+      <c r="D30" s="12">
         <v>3.8516533109776918</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="12">
         <v>3.7581543956424142</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="12">
         <v>-12.036887229000438</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="12">
         <v>4.184233345994083</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="12">
         <v>-10.9149002429796</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I30" s="12">
         <v>-3.4293394173311591</v>
       </c>
-      <c r="J30" s="2">
+      <c r="J30" s="12">
         <v>-17.629879402576066</v>
       </c>
-      <c r="K30" s="2">
+      <c r="K30" s="12">
         <v>6.3830266341498287</v>
       </c>
-      <c r="L30" s="2">
+      <c r="L30" s="12">
         <v>-51.659719587409143</v>
       </c>
-      <c r="M30" s="2">
-        <v>-68.489999999999995</v>
-      </c>
-      <c r="N30" s="2">
+      <c r="M30" s="12">
+        <v>-68.489999999999995</v>
+      </c>
+      <c r="N30" s="12">
         <v>28.474498581447751</v>
       </c>
-      <c r="O30" s="2">
+      <c r="O30" s="12">
         <v>7.5556536366143394</v>
       </c>
-      <c r="P30" s="2">
+      <c r="P30" s="12">
         <v>27.558334711477976</v>
       </c>
-      <c r="Q30" s="2">
+      <c r="Q30" s="12">
         <v>3.8685960673635758</v>
       </c>
-      <c r="R30" s="2">
+      <c r="R30" s="12">
         <v>5.003760753065162</v>
       </c>
-      <c r="S30" s="2">
+      <c r="S30" s="13">
         <v>-42.804305523508965</v>
       </c>
-      <c r="T30" s="2">
+      <c r="T30" s="12">
         <v>-25.779972788544853</v>
       </c>
-      <c r="U30">
+      <c r="U30" s="11">
         <v>-62.54</v>
       </c>
     </row>
@@ -2609,7 +2668,7 @@
       <c r="R31" s="2">
         <v>12.053202476101925</v>
       </c>
-      <c r="S31" s="2">
+      <c r="S31" s="9">
         <v>-35.762393914453192</v>
       </c>
       <c r="T31" s="2">
@@ -2674,7 +2733,7 @@
       <c r="R32" s="2">
         <v>20.72099119961911</v>
       </c>
-      <c r="S32" s="2">
+      <c r="S32" s="9">
         <v>-30.207679820780299</v>
       </c>
       <c r="T32" s="2">
@@ -2684,7 +2743,7 @@
         <v>-62.54</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -2739,7 +2798,7 @@
       <c r="R33" s="2">
         <v>18.948276862100393</v>
       </c>
-      <c r="S33" s="2">
+      <c r="S33" s="9">
         <v>-31.881875166548379</v>
       </c>
       <c r="T33" s="2">
@@ -2749,7 +2808,7 @@
         <v>-62.54</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -2804,7 +2863,7 @@
       <c r="R34" s="2">
         <v>12.912262981359175</v>
       </c>
-      <c r="S34" s="2">
+      <c r="S34" s="9">
         <v>-35.684582736649645</v>
       </c>
       <c r="T34" s="2">
@@ -2814,7 +2873,7 @@
         <v>-62.54</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -2869,7 +2928,7 @@
       <c r="R35" s="2">
         <v>12.631766235496022</v>
       </c>
-      <c r="S35" s="2">
+      <c r="S35" s="9">
         <v>-39.420774299205455</v>
       </c>
       <c r="T35" s="2">
@@ -2879,72 +2938,72 @@
         <v>-62.54</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B36">
-        <v>0</v>
-      </c>
-      <c r="C36" s="2">
-        <v>27.629243285012969</v>
-      </c>
-      <c r="D36" s="2">
+      <c r="B36" s="4">
+        <v>0</v>
+      </c>
+      <c r="C36" s="5">
+        <v>27.629243285012969</v>
+      </c>
+      <c r="D36" s="5">
         <v>2.5062729429501514</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="5">
         <v>4.5168133812958322</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F36" s="5">
         <v>-12.28663600979792</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G36" s="5">
         <v>9.3473815120848673</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H36" s="5">
         <v>-8.4763983257156639</v>
       </c>
-      <c r="I36" s="2">
+      <c r="I36" s="5">
         <v>-0.21398073945912757</v>
       </c>
-      <c r="J36" s="2">
+      <c r="J36" s="5">
         <v>-17.486179726939493</v>
       </c>
-      <c r="K36" s="2">
+      <c r="K36" s="5">
         <v>14.195519908972223</v>
       </c>
-      <c r="L36" s="2">
+      <c r="L36" s="5">
         <v>-58.975225338344877</v>
       </c>
-      <c r="M36" s="2">
-        <v>-68.489999999999995</v>
-      </c>
-      <c r="N36" s="2">
+      <c r="M36" s="5">
+        <v>-68.489999999999995</v>
+      </c>
+      <c r="N36" s="5">
         <v>27.33807887703469</v>
       </c>
-      <c r="O36" s="2">
+      <c r="O36" s="5">
         <v>6.3019837820691782</v>
       </c>
-      <c r="P36" s="2">
+      <c r="P36" s="5">
         <v>26.022191455646706</v>
       </c>
-      <c r="Q36" s="2">
+      <c r="Q36" s="5">
         <v>-7.5439192089297604</v>
       </c>
-      <c r="R36" s="2">
+      <c r="R36" s="5">
         <v>10.109178045301704</v>
       </c>
-      <c r="S36" s="2">
+      <c r="S36" s="3">
         <v>-43.088567326790653</v>
       </c>
-      <c r="T36" s="2">
+      <c r="T36" s="5">
         <v>-23.911249497554515</v>
       </c>
-      <c r="U36">
-        <v>-62.54</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U36" s="4">
+        <v>-62.54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -2999,7 +3058,7 @@
       <c r="R37" s="2">
         <v>16.711833003754347</v>
       </c>
-      <c r="S37" s="2">
+      <c r="S37" s="9">
         <v>-28.304443507020398</v>
       </c>
       <c r="T37" s="2">
@@ -3009,7 +3068,7 @@
         <v>-62.54</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -3064,7 +3123,7 @@
       <c r="R38" s="2">
         <v>15.557843033813684</v>
       </c>
-      <c r="S38" s="2">
+      <c r="S38" s="9">
         <v>-32.916010822220301</v>
       </c>
       <c r="T38" s="2">
@@ -3074,7 +3133,7 @@
         <v>-62.54</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -3129,7 +3188,7 @@
       <c r="R39" s="2">
         <v>21.172170529907408</v>
       </c>
-      <c r="S39" s="2">
+      <c r="S39" s="9">
         <v>-26.554319511444646</v>
       </c>
       <c r="T39" s="2">
@@ -3139,7 +3198,7 @@
         <v>-62.54</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -3194,7 +3253,7 @@
       <c r="R40" s="2">
         <v>16.754503649931969</v>
       </c>
-      <c r="S40" s="2">
+      <c r="S40" s="9">
         <v>-26.029721569627693</v>
       </c>
       <c r="T40" s="2">
@@ -3204,7 +3263,7 @@
         <v>-62.54</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>50</v>
       </c>
@@ -3259,7 +3318,7 @@
       <c r="R41" s="2">
         <v>19.65171501175055</v>
       </c>
-      <c r="S41" s="2">
+      <c r="S41" s="9">
         <v>-30.957553672885179</v>
       </c>
       <c r="T41" s="2">
@@ -3269,72 +3328,73 @@
         <v>-62.54</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>51</v>
       </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
-      <c r="C42" s="2">
-        <v>27.629243285012969</v>
-      </c>
-      <c r="D42" s="2">
+      <c r="B42" s="14">
+        <v>0</v>
+      </c>
+      <c r="C42" s="9">
+        <v>27.629243285012969</v>
+      </c>
+      <c r="D42" s="9">
         <v>2.8131250888881967</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42" s="9">
         <v>4.1421902098142507</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F42" s="17">
         <v>-11.164021514064649</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42" s="9">
         <v>20.133014798248158</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42" s="9">
         <v>-0.39156592786746591</v>
       </c>
-      <c r="I42" s="2">
+      <c r="I42" s="9">
         <v>1.6164644721991939</v>
       </c>
-      <c r="J42" s="2">
+      <c r="J42" s="9">
         <v>-12.973131402919515</v>
       </c>
-      <c r="K42" s="2">
+      <c r="K42" s="9">
         <v>13.606915998174191</v>
       </c>
-      <c r="L42" s="2">
+      <c r="L42" s="9">
         <v>-59.363653718791603</v>
       </c>
-      <c r="M42" s="2">
-        <v>-68.489999999999995</v>
-      </c>
-      <c r="N42" s="2">
+      <c r="M42" s="9">
+        <v>-68.489999999999995</v>
+      </c>
+      <c r="N42" s="9">
         <v>27.227637204885493</v>
       </c>
-      <c r="O42" s="2">
+      <c r="O42" s="9">
         <v>7.8997170954588718</v>
       </c>
-      <c r="P42" s="2">
+      <c r="P42" s="9">
         <v>28.754367818454543</v>
       </c>
-      <c r="Q42" s="2">
+      <c r="Q42" s="9">
         <v>1.5060227961976579E-2</v>
       </c>
-      <c r="R42" s="2">
+      <c r="R42" s="9">
         <v>8.8259211176886563</v>
       </c>
-      <c r="S42" s="2">
+      <c r="S42" s="9">
         <v>-34.843720006489754</v>
       </c>
-      <c r="T42" s="2">
+      <c r="T42" s="9">
         <v>-21.131382412581726</v>
       </c>
-      <c r="U42">
-        <v>-62.54</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U42" s="14">
+        <v>-62.54</v>
+      </c>
+      <c r="V42" s="14"/>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -3389,7 +3449,7 @@
       <c r="R43" s="2">
         <v>14.201795004099058</v>
       </c>
-      <c r="S43" s="2">
+      <c r="S43" s="9">
         <v>-32.165509460402987</v>
       </c>
       <c r="T43" s="2">

</xml_diff>